<commit_message>
pin map initial commit & update
</commit_message>
<xml_diff>
--- a/Connectors/M7.9.7/Bosch_M797_pinout.xlsx
+++ b/Connectors/M7.9.7/Bosch_M797_pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="131">
   <si>
     <t>№</t>
   </si>
@@ -156,60 +156,27 @@
     <t>Ignition Switch KL15</t>
   </si>
   <si>
-    <t>Engine Speed</t>
-  </si>
-  <si>
     <t>K-Line (Tester)</t>
   </si>
   <si>
     <t>K-Line (Immobiliser)</t>
   </si>
   <si>
-    <t>Phase Sensor</t>
-  </si>
-  <si>
     <t>Vehicle speed</t>
   </si>
   <si>
     <t>A/C Kompressor Switch</t>
   </si>
   <si>
-    <t>Inertia switch (crash detection)</t>
-  </si>
-  <si>
-    <t>Power Steering</t>
-  </si>
-  <si>
-    <t>A/C Switch</t>
-  </si>
-  <si>
-    <t>Clutch switch</t>
-  </si>
-  <si>
     <t>Reserve (PWM-alternator)</t>
   </si>
   <si>
-    <t>Engine Coolant Temperature</t>
-  </si>
-  <si>
-    <t>Intake Air Temperature</t>
-  </si>
-  <si>
-    <t>Throttle Position Sensor</t>
-  </si>
-  <si>
     <t>Fan Diagnostic</t>
   </si>
   <si>
     <t>Manifold pressure</t>
   </si>
   <si>
-    <t>Lambda Sensor Upstream</t>
-  </si>
-  <si>
-    <t>Lambda Sensor Downstream</t>
-  </si>
-  <si>
     <t>Knock Sensor (-)</t>
   </si>
   <si>
@@ -219,9 +186,6 @@
     <t>Reserve (fuel level)</t>
   </si>
   <si>
-    <t>Reserve (fuel level ground)</t>
-  </si>
-  <si>
     <t>power ground</t>
   </si>
   <si>
@@ -234,15 +198,9 @@
     <t>Main Relay</t>
   </si>
   <si>
-    <t>Engine Speed Signal (10mA)</t>
-  </si>
-  <si>
     <t>Reserve (PWM-Fuel level)</t>
   </si>
   <si>
-    <t>Reserve (Fuel consumption)</t>
-  </si>
-  <si>
     <t>Injector Valve 1 (Cyl 1)</t>
   </si>
   <si>
@@ -255,27 +213,9 @@
     <t>Injector Valve 4 (Cyl 2)</t>
   </si>
   <si>
-    <t>Cooling Fan Relay (High Speed)</t>
-  </si>
-  <si>
-    <t>Reserve</t>
-  </si>
-  <si>
     <t>MIL Lamp</t>
   </si>
   <si>
-    <t>Reserve (LSF Heating Downstream)</t>
-  </si>
-  <si>
-    <t>Canister Purge Valve</t>
-  </si>
-  <si>
-    <t>LSF Heating Upstream</t>
-  </si>
-  <si>
-    <t>Cooling Fan Relay (Low Speed)</t>
-  </si>
-  <si>
     <t>HOT Lamp</t>
   </si>
   <si>
@@ -285,21 +225,6 @@
     <t>Fuel Pump Relay</t>
   </si>
   <si>
-    <t>Stepper A</t>
-  </si>
-  <si>
-    <t>Stepper D</t>
-  </si>
-  <si>
-    <t>Stepper C</t>
-  </si>
-  <si>
-    <t>Stepper B</t>
-  </si>
-  <si>
-    <t>Ignition 1</t>
-  </si>
-  <si>
     <t>Ignition 2</t>
   </si>
   <si>
@@ -366,15 +291,6 @@
     <t>IN_analog</t>
   </si>
   <si>
-    <t>V_REF</t>
-  </si>
-  <si>
-    <t>? IN_divided?</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>K-LINE</t>
   </si>
   <si>
@@ -388,13 +304,118 @@
   </si>
   <si>
     <t>STEPPER_B</t>
+  </si>
+  <si>
+    <t>VIGN</t>
+  </si>
+  <si>
+    <t>V12</t>
+  </si>
+  <si>
+    <t>OUT12_FAST</t>
+  </si>
+  <si>
+    <t>V5</t>
+  </si>
+  <si>
+    <t>V_REF2</t>
+  </si>
+  <si>
+    <t>V_REF1</t>
+  </si>
+  <si>
+    <t>Ignition 2-3 or 3</t>
+  </si>
+  <si>
+    <t>Ignition 1-4 or 1</t>
+  </si>
+  <si>
+    <t>Ignition 4</t>
+  </si>
+  <si>
+    <t>Engine Speed (Tach) Signal</t>
+  </si>
+  <si>
+    <t>Reserve (LSF Heating Out)</t>
+  </si>
+  <si>
+    <t>Lambda Sensor In</t>
+  </si>
+  <si>
+    <t>Reserve (fuel level gnd)</t>
+  </si>
+  <si>
+    <t>ECF Relay 2 (High Speed)</t>
+  </si>
+  <si>
+    <t>ECF Relay 1 (Low Speed)</t>
+  </si>
+  <si>
+    <t>Inertia switch (crash detect)</t>
+  </si>
+  <si>
+    <t>Fuel consumption</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Throttle Position Sensor (TPS)</t>
+  </si>
+  <si>
+    <t>Reserve (out)</t>
+  </si>
+  <si>
+    <t>CheckEngine Lamp (low)</t>
+  </si>
+  <si>
+    <t>Engine Speed (Crank sensor -)</t>
+  </si>
+  <si>
+    <t>Engine Speed (Crank sensor +)</t>
+  </si>
+  <si>
+    <t>Engine Coolant Temp. (CLT)</t>
+  </si>
+  <si>
+    <t>Intake Air Temperature (IAT)</t>
+  </si>
+  <si>
+    <t>Canister Purge Valve (out)</t>
+  </si>
+  <si>
+    <t>O2 LSF Heating Output</t>
+  </si>
+  <si>
+    <t>Stepper A (or D)</t>
+  </si>
+  <si>
+    <t>Stepper D (or C)</t>
+  </si>
+  <si>
+    <t>Stepper C (or B)</t>
+  </si>
+  <si>
+    <t>Stepper B (or A)</t>
+  </si>
+  <si>
+    <t>A/C Switch (in)</t>
+  </si>
+  <si>
+    <t>Power Steering (in)</t>
+  </si>
+  <si>
+    <t>Clutch switch (in?)</t>
+  </si>
+  <si>
+    <t>Phase Sensor Input</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +435,15 @@
     </font>
     <font>
       <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,10 +473,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -750,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,8 +801,11 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="C3" t="s">
+        <v>69</v>
+      </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -779,10 +813,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="D4" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,10 +824,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
         <v>1</v>
@@ -803,8 +837,11 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="C6" t="s">
+        <v>104</v>
+      </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -812,10 +849,10 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -823,13 +860,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -837,13 +874,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -854,7 +891,7 @@
         <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="D10" t="s">
         <v>2</v>
@@ -865,15 +902,18 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="D12" t="s">
         <v>3</v>
@@ -888,6 +928,9 @@
       <c r="A14">
         <v>12</v>
       </c>
+      <c r="B14" t="s">
+        <v>113</v>
+      </c>
       <c r="C14" t="s">
         <v>43</v>
       </c>
@@ -899,6 +942,9 @@
       <c r="A15">
         <v>13</v>
       </c>
+      <c r="B15" t="s">
+        <v>96</v>
+      </c>
       <c r="C15" t="s">
         <v>45</v>
       </c>
@@ -911,10 +957,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
@@ -925,10 +971,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -939,10 +985,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C18" t="s">
-        <v>59</v>
+        <v>114</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -953,10 +999,10 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
       <c r="D19" t="s">
         <v>34</v>
@@ -967,10 +1013,10 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="D20" t="s">
         <v>8</v>
@@ -981,10 +1027,10 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="D21" t="s">
         <v>9</v>
@@ -995,10 +1041,10 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="C22" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D22" t="s">
         <v>10</v>
@@ -1019,10 +1065,10 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C25" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1030,13 +1076,19 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>115</v>
+      </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
@@ -1045,8 +1097,11 @@
       <c r="A28">
         <v>26</v>
       </c>
+      <c r="B28" t="s">
+        <v>98</v>
+      </c>
       <c r="C28" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
         <v>11</v>
@@ -1057,21 +1112,24 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
+      <c r="B30" t="s">
+        <v>74</v>
+      </c>
       <c r="C30" t="s">
-        <v>82</v>
+        <v>106</v>
       </c>
       <c r="D30" t="s">
         <v>38</v>
@@ -1082,10 +1140,10 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C31" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="D31" t="s">
         <v>39</v>
@@ -1101,7 +1159,10 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>74</v>
+      </c>
+      <c r="C33" t="s">
+        <v>116</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -1111,8 +1172,11 @@
       <c r="A34">
         <v>32</v>
       </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
       <c r="C34" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="D34" t="s">
         <v>35</v>
@@ -1122,8 +1186,11 @@
       <c r="A35">
         <v>33</v>
       </c>
+      <c r="B35" t="s">
+        <v>99</v>
+      </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="D35" t="s">
         <v>13</v>
@@ -1134,10 +1201,10 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="C36" t="s">
-        <v>46</v>
+        <v>117</v>
       </c>
       <c r="D36" t="s">
         <v>14</v>
@@ -1148,10 +1215,10 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="D37" t="s">
         <v>36</v>
@@ -1162,10 +1229,10 @@
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="D38" t="s">
         <v>15</v>
@@ -1176,10 +1243,10 @@
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D39" t="s">
         <v>16</v>
@@ -1195,10 +1262,10 @@
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C41" t="s">
-        <v>57</v>
+        <v>119</v>
       </c>
       <c r="D41" t="s">
         <v>17</v>
@@ -1209,10 +1276,10 @@
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C42" t="s">
-        <v>58</v>
+        <v>120</v>
       </c>
       <c r="D42" t="s">
         <v>18</v>
@@ -1228,10 +1295,10 @@
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
         <v>40</v>
@@ -1247,7 +1314,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="C46" t="s">
         <v>44</v>
@@ -1261,7 +1328,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C47" t="s">
         <v>44</v>
@@ -1275,10 +1342,10 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C48" t="s">
-        <v>83</v>
+        <v>121</v>
       </c>
       <c r="D48" t="s">
         <v>21</v>
@@ -1289,13 +1356,13 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="D49" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,10 +1370,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="D50" t="s">
         <v>22</v>
@@ -1322,10 +1389,10 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C52" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D52" t="s">
         <v>23</v>
@@ -1336,10 +1403,10 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D53" t="s">
         <v>24</v>
@@ -1350,7 +1417,7 @@
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,10 +1425,10 @@
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C55" t="s">
-        <v>67</v>
+        <v>108</v>
       </c>
       <c r="D55" t="s">
         <v>24</v>
@@ -1377,10 +1444,10 @@
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="C57" t="s">
-        <v>63</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
         <v>42</v>
@@ -1396,7 +1463,7 @@
         <v>57</v>
       </c>
       <c r="D59" t="s">
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1404,7 +1471,7 @@
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1412,10 +1479,10 @@
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C61" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D61" t="s">
         <v>25</v>
@@ -1431,10 +1498,10 @@
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D63" t="s">
         <v>26</v>
@@ -1449,6 +1516,9 @@
       <c r="A65">
         <v>63</v>
       </c>
+      <c r="B65" t="s">
+        <v>97</v>
+      </c>
       <c r="C65" t="s">
         <v>44</v>
       </c>
@@ -1461,10 +1531,10 @@
         <v>64</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>120</v>
+        <v>92</v>
       </c>
       <c r="C66" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="D66" t="s">
         <v>27</v>
@@ -1475,10 +1545,10 @@
         <v>65</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="C67" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="D67" t="s">
         <v>28</v>
@@ -1489,10 +1559,10 @@
         <v>66</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>122</v>
+        <v>94</v>
       </c>
       <c r="C68" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="D68" t="s">
         <v>29</v>
@@ -1503,10 +1573,10 @@
         <v>67</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>123</v>
+        <v>95</v>
       </c>
       <c r="C69" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="D69" t="s">
         <v>30</v>
@@ -1517,13 +1587,13 @@
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C70" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D70" t="s">
-        <v>101</v>
+        <v>76</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1531,13 +1601,13 @@
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C71" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D71" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1545,13 +1615,13 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>74</v>
       </c>
       <c r="C72" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="D72" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1559,10 +1629,10 @@
         <v>71</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="C73" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D73" t="s">
         <v>31</v>
@@ -1573,7 +1643,7 @@
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -1586,7 +1656,7 @@
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -1594,13 +1664,13 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C77" t="s">
-        <v>54</v>
+        <v>127</v>
       </c>
       <c r="D77" t="s">
-        <v>104</v>
+        <v>79</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -1608,13 +1678,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C78" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="D78" t="s">
-        <v>105</v>
+        <v>80</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -1622,10 +1692,10 @@
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>114</v>
-      </c>
-      <c r="C79" t="s">
-        <v>55</v>
+        <v>89</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1638,10 +1708,10 @@
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>114</v>
+        <v>89</v>
       </c>
       <c r="C81" t="s">
-        <v>49</v>
+        <v>130</v>
       </c>
       <c r="D81" t="s">
         <v>32</v>
@@ -1652,10 +1722,10 @@
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>95</v>
+        <v>70</v>
       </c>
       <c r="C82" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="D82" t="s">
         <v>26</v>

</xml_diff>